<commit_message>
start code for generate qcm
</commit_message>
<xml_diff>
--- a/exemple.xlsx
+++ b/exemple.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LeweenH\PycharmProjects\QCM_al-atoires\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{DB3AC7E2-DDB9-4DBD-A895-F605EDF21756}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A5D0C86-4347-4F84-BD12-81A52B795317}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="exemple" sheetId="1" r:id="rId1"/>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -920,10 +920,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
@@ -1065,10 +1065,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
optimize quest_&_answ_randomizer.py + randomize answers
</commit_message>
<xml_diff>
--- a/exemple.xlsx
+++ b/exemple.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LeweenH\PycharmProjects\QCM_al-atoires\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lewee\PycharmProjects\QCM_aleatoires\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A5D0C86-4347-4F84-BD12-81A52B795317}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F0733FC-6639-46AD-B51A-A5AB95F14B52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="exemple" sheetId="1" r:id="rId1"/>
@@ -21,23 +21,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>Question 1</t>
   </si>
   <si>
-    <t>Reponse 1</t>
-  </si>
-  <si>
-    <t>Reponse 2</t>
-  </si>
-  <si>
-    <t>Reponse 3</t>
-  </si>
-  <si>
-    <t>Reponse 4</t>
-  </si>
-  <si>
     <t>Question 2</t>
   </si>
   <si>
@@ -50,31 +38,139 @@
     <t>Question 5</t>
   </si>
   <si>
-    <t>Question 1-2</t>
-  </si>
-  <si>
-    <t>Reponse 12</t>
-  </si>
-  <si>
-    <t>Reponse 22</t>
-  </si>
-  <si>
-    <t>Reponse 32</t>
-  </si>
-  <si>
-    <t>Reponse 42</t>
-  </si>
-  <si>
-    <t>Question 2-2</t>
-  </si>
-  <si>
-    <t>Question 3-2</t>
-  </si>
-  <si>
-    <t>Question 4-2</t>
-  </si>
-  <si>
-    <t>Question 5-2</t>
+    <t>Reponse 1-2</t>
+  </si>
+  <si>
+    <t>Reponse 2-2</t>
+  </si>
+  <si>
+    <t>Reponse 1-3</t>
+  </si>
+  <si>
+    <t>Reponse 2-3</t>
+  </si>
+  <si>
+    <t>Reponse 3-2</t>
+  </si>
+  <si>
+    <t>Reponse 4-2</t>
+  </si>
+  <si>
+    <t>Reponse 3-3</t>
+  </si>
+  <si>
+    <t>Reponse 4-3</t>
+  </si>
+  <si>
+    <t>Reponse 1-4</t>
+  </si>
+  <si>
+    <t>Reponse 2-4</t>
+  </si>
+  <si>
+    <t>Reponse 3-4</t>
+  </si>
+  <si>
+    <t>Reponse 4-4</t>
+  </si>
+  <si>
+    <t>Reponse 1-5</t>
+  </si>
+  <si>
+    <t>Reponse 2-5</t>
+  </si>
+  <si>
+    <t>Reponse 3-5</t>
+  </si>
+  <si>
+    <t>Reponse 4-5</t>
+  </si>
+  <si>
+    <t>Question 12</t>
+  </si>
+  <si>
+    <t>Question 22</t>
+  </si>
+  <si>
+    <t>Question 33</t>
+  </si>
+  <si>
+    <t>Question 44</t>
+  </si>
+  <si>
+    <t>Question 55</t>
+  </si>
+  <si>
+    <t>Reponse 1-1</t>
+  </si>
+  <si>
+    <t>Reponse 2-1</t>
+  </si>
+  <si>
+    <t>Reponse 3-1</t>
+  </si>
+  <si>
+    <t>Reponse 4-1</t>
+  </si>
+  <si>
+    <t>Reponse 12-1</t>
+  </si>
+  <si>
+    <t>Reponse 22-1</t>
+  </si>
+  <si>
+    <t>Reponse 32-1</t>
+  </si>
+  <si>
+    <t>Reponse 42-1</t>
+  </si>
+  <si>
+    <t>Reponse 12-2</t>
+  </si>
+  <si>
+    <t>Reponse 22-2</t>
+  </si>
+  <si>
+    <t>Reponse 32-2</t>
+  </si>
+  <si>
+    <t>Reponse 42-2</t>
+  </si>
+  <si>
+    <t>Reponse 12-3</t>
+  </si>
+  <si>
+    <t>Reponse 22-3</t>
+  </si>
+  <si>
+    <t>Reponse 32-3</t>
+  </si>
+  <si>
+    <t>Reponse 42-3</t>
+  </si>
+  <si>
+    <t>Reponse 12-4</t>
+  </si>
+  <si>
+    <t>Reponse 22-4</t>
+  </si>
+  <si>
+    <t>Reponse 32-4</t>
+  </si>
+  <si>
+    <t>Reponse 12-5</t>
+  </si>
+  <si>
+    <t>Reponse 22-5</t>
+  </si>
+  <si>
+    <t>Reponse 32-5</t>
+  </si>
+  <si>
+    <t>Reponse 42-5</t>
+  </si>
+  <si>
+    <t>Reponse 42-4</t>
   </si>
 </sst>
 </file>
@@ -923,11 +1019,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="25.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1">
@@ -937,22 +1036,22 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -960,25 +1059,25 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
         <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -986,25 +1085,25 @@
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1012,25 +1111,25 @@
         <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -1038,28 +1137,29 @@
         <v>5</v>
       </c>
       <c r="B17" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C17" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1068,13 +1168,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1082,25 +1183,25 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C1" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1108,25 +1209,25 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1134,25 +1235,25 @@
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1160,25 +1261,25 @@
         <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="C13" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>11</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
-        <v>13</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -1186,25 +1287,25 @@
         <v>5</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="C17" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>12</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change exemple change file_name add exemple.csv for compare docx files finished generate qcm file
</commit_message>
<xml_diff>
--- a/exemple.xlsx
+++ b/exemple.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lewee\PycharmProjects\QCM_aleatoires\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F0733FC-6639-46AD-B51A-A5AB95F14B52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5830D496-D144-43B8-8376-1BB88A42BD3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="exemple" sheetId="1" r:id="rId1"/>
@@ -1019,8 +1019,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1168,7 +1168,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>

</xml_diff>